<commit_message>
testes de extracao ok
</commit_message>
<xml_diff>
--- a/streamlit/dados_brutos/homegate_alugar_geneve_20240815.xlsx
+++ b/streamlit/dados_brutos/homegate_alugar_geneve_20240815.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,7 +503,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:12</t>
+          <t>2024-08-15 21:51:18</t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:13</t>
+          <t>2024-08-15 21:51:19</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:14</t>
+          <t>2024-08-15 21:51:20</t>
         </is>
       </c>
     </row>
@@ -614,7 +614,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:15</t>
+          <t>2024-08-15 21:51:22</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:16</t>
+          <t>2024-08-15 21:51:23</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:17</t>
+          <t>2024-08-15 21:51:24</t>
         </is>
       </c>
     </row>
@@ -725,7 +725,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:18</t>
+          <t>2024-08-15 21:51:25</t>
         </is>
       </c>
     </row>
@@ -762,7 +762,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:19</t>
+          <t>2024-08-15 21:51:26</t>
         </is>
       </c>
     </row>
@@ -799,7 +799,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:21</t>
+          <t>2024-08-15 21:51:27</t>
         </is>
       </c>
     </row>
@@ -836,7 +836,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:22</t>
+          <t>2024-08-15 21:51:28</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:23</t>
+          <t>2024-08-15 21:51:29</t>
         </is>
       </c>
     </row>
@@ -910,7 +910,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:24</t>
+          <t>2024-08-15 21:51:30</t>
         </is>
       </c>
     </row>
@@ -947,7 +947,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:25</t>
+          <t>2024-08-15 21:51:31</t>
         </is>
       </c>
     </row>
@@ -984,7 +984,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:26</t>
+          <t>2024-08-15 21:51:32</t>
         </is>
       </c>
     </row>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:27</t>
+          <t>2024-08-15 21:51:33</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:28</t>
+          <t>2024-08-15 21:51:35</t>
         </is>
       </c>
     </row>
@@ -1095,7 +1095,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:29</t>
+          <t>2024-08-15 21:51:36</t>
         </is>
       </c>
     </row>
@@ -1132,7 +1132,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:30</t>
+          <t>2024-08-15 21:51:37</t>
         </is>
       </c>
     </row>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:31</t>
+          <t>2024-08-15 21:51:38</t>
         </is>
       </c>
     </row>
@@ -1206,7 +1206,747 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2024-08-15 21:25:32</t>
+          <t>2024-08-15 21:51:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Appartement à Genève</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CHF 1,430.– / month</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>25m²</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Rue de la Navigation, 1201 Genève</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001355523</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Studio à Genève - meublé - piscine - proche des organisations internationales</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>CHF 1,760.– / month</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>26m²</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Avenue De-Budé, 1202 Genève</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001352171</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Appartement à Genève</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>CHF 1,500.– / month</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>25m²</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Rue Louise-De-Frotté 35, 1205 Genève</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001337045</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>City-Penthouse en plein coeur des rues basses</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>CHF 4,850.– / month</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>100m²</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Rue de la Croix-d'Or 27, 1204 Genève</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001335811</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Appartement en campagne</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>CHF 2,210.– / month</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>78m²</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Route de Mon-Idée 49, 1226 Thônex</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001333875</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Appartement à Thônex</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>CHF 4,564.– / month</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>139m²</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Cour de l'Emine 1, 1226 Thônex</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001328477</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Splendide logement dans le prestigieux quartier de Champel</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>CHF 2,900.– / month</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>69m²</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Rue de Contamines 35, 1206 Genève</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001313855</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>5 pièces de haute qualité architecturale, centre ville</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>CHF 4,250.– / month</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>100m²</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Avenue de Frontenex 4, 1207 Genève</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001313160</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Appartement de 5.5 pièces meublé à Thônex</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>CHF 3,900.– / month</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>5.5</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>130m²</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Chemin Etienne-Chennaz 15, 1226 Thônex</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001308653</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Spacious, peaceful, nicely furnished Apartment close to the UN</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CHF 4,775.– / month</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>120m²</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Chemin du Point-du-Jour, 1202 Geneva</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001305957</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Splendide logement dans le prestigieux quartier de Champel</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CHF 2,850.– / month</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>80m²</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Rue de Contamines 35, 1206 Genève</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001287129</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Beau logement 4.5 pièces très spacieux proche de Cornavin / Mercier</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CHF 2,920.– / month</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Rue Jean-Gutenberg, 1201 Genève</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001271361</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Appartement à Genève</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CHF 1,270.– / month</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>30m²</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Rue Jean-Charles Amat 15, 1202 Genève</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001243823</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Splendide logement dans le quartier de Champel</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>CHF 2,750.– / month</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>63m²</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Rue de Contamines 35, 1206 Genève</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001232755</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Studio à Chêne-Bougeries</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>CHF 1,690.– / month</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>28m²</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Avenue Pierre-Odier, 1224 Chêne-Bougeries</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001178602</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Appartement à Genève</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>CHF 1,600.– / month</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>60m²</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Rue de Contamines, 1206 Genève</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001158284</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Appartement de charme dans le vieux Chêne-Bourg</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>CHF 2,090.– / month</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2.5</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>56m²</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Rue du Gothard 7, 1225 Chêne-Bourg</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4000848882</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Bel appartement lumineux</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CHF 2,255.– / month</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>65m²</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Rue des Bossons 26, 1213 Onex</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/3003397551</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Magnifique appartement au centre-ville de Genève ! Terme fixe au 31.08.2026</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>CHF 4,870.– / month</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>105m²</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Rue Charles-Giron 14, 1203 Genève</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4001225099</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Un projet unique au coeur de Genève</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>CHF 5,460.– / month</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>104m²</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Rue du Vieux Collège 3, 1204 Genève</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>https://www.homegate.ch/rent/4000656611</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2024-08-15 21:52:20</t>
         </is>
       </c>
     </row>

</xml_diff>